<commit_message>
feat: Tipos de gastos, carga
</commit_message>
<xml_diff>
--- a/src/Conceptos/Plantillas carga de datos.xlsx
+++ b/src/Conceptos/Plantillas carga de datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseLuisPerezOlguin\Documents\praxia-excel\src\Conceptos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB7F2E42-548E-474D-870E-AF6870B62234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194C5AE4-68EE-4EA8-B8E0-FE73FD039A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11160" activeTab="1" xr2:uid="{08F850AA-7DE7-4012-8361-B83FCF36AA13}"/>
   </bookViews>
@@ -5026,25 +5026,25 @@
   </sheetPr>
   <dimension ref="A1:BL1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AH17" sqref="AH17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="18" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="6.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="22" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="29.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="5.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="6.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="2.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="17.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="9.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="10.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="18" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="20.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="6.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="15.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="22" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="29.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="10.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="5.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" style="26" customWidth="1" outlineLevel="1"/>
     <col min="16" max="16" width="24.85546875" style="24" customWidth="1" outlineLevel="1"/>
@@ -5059,9 +5059,10 @@
     <col min="26" max="26" width="9" style="10" customWidth="1" outlineLevel="1"/>
     <col min="27" max="27" width="14" customWidth="1" outlineLevel="1"/>
     <col min="28" max="28" width="9" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="9" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="14" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="44" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="9.140625" collapsed="1"/>
+    <col min="30" max="30" width="9" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="14" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="44" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="34" max="34" width="9" customWidth="1" outlineLevel="1"/>
     <col min="35" max="35" width="23.42578125" customWidth="1" outlineLevel="1"/>
     <col min="36" max="36" width="9" customWidth="1" outlineLevel="1"/>
@@ -7179,7 +7180,7 @@
         <v>381</v>
       </c>
       <c r="AH16" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AI16" s="6" t="s">
         <v>304</v>

</xml_diff>